<commit_message>
adaugare analitice predictive, inca nu merge complet, mai necesita modificari
</commit_message>
<xml_diff>
--- a/backend/ExportedData.xlsx
+++ b/backend/ExportedData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -52,34 +52,127 @@
     <t>Sales Change (%)</t>
   </si>
   <si>
-    <t>2022-04-01</t>
+    <t>2023-04-01</t>
+  </si>
+  <si>
+    <t>Nails</t>
+  </si>
+  <si>
+    <t>Top coat</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>23-32</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Transylvania</t>
+  </si>
+  <si>
+    <t>███████    22</t>
+  </si>
+  <si>
+    <t>▲ 90.00%</t>
+  </si>
+  <si>
+    <t>Fragrance</t>
+  </si>
+  <si>
+    <t>Pocket perfume</t>
+  </si>
+  <si>
+    <t>Youth</t>
+  </si>
+  <si>
+    <t>63-73</t>
+  </si>
+  <si>
+    <t>██████     18</t>
+  </si>
+  <si>
+    <t>▲ 201.06%</t>
+  </si>
+  <si>
+    <t>Lips</t>
+  </si>
+  <si>
+    <t>Lip liner</t>
+  </si>
+  <si>
+    <t>Seniors</t>
+  </si>
+  <si>
+    <t>████       11</t>
+  </si>
+  <si>
+    <t>▲ 137.40%</t>
+  </si>
+  <si>
+    <t>Skincare</t>
+  </si>
+  <si>
+    <t>Moisturizing</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>13-22</t>
+  </si>
+  <si>
+    <t>█████      16</t>
+  </si>
+  <si>
+    <t>▼ -53.14%</t>
+  </si>
+  <si>
+    <t>Makeup</t>
+  </si>
+  <si>
+    <t>Lipstick</t>
+  </si>
+  <si>
+    <t>53-62</t>
+  </si>
+  <si>
+    <t>██████     19</t>
+  </si>
+  <si>
+    <t>▲ 320.84%</t>
   </si>
   <si>
     <t>Hands</t>
   </si>
   <si>
-    <t>Repair lotion</t>
-  </si>
-  <si>
-    <t>Seniors</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>53-62</t>
-  </si>
-  <si>
-    <t>Romania</t>
-  </si>
-  <si>
-    <t>Ardeal</t>
-  </si>
-  <si>
-    <t>█████      14</t>
-  </si>
-  <si>
-    <t>▼ -43.34%</t>
+    <t>Liquid soap</t>
+  </si>
+  <si>
+    <t>33-42</t>
+  </si>
+  <si>
+    <t>█████████  29</t>
+  </si>
+  <si>
+    <t>▲ 201.79%</t>
+  </si>
+  <si>
+    <t>Hand cream</t>
+  </si>
+  <si>
+    <t>43-52</t>
+  </si>
+  <si>
+    <t>█████      15</t>
+  </si>
+  <si>
+    <t>➔ -7.02%</t>
   </si>
   <si>
     <t>Eyes</t>
@@ -88,130 +181,19 @@
     <t>Mascara</t>
   </si>
   <si>
-    <t>Children</t>
-  </si>
-  <si>
-    <t>63-73</t>
-  </si>
-  <si>
-    <t>███████    18</t>
-  </si>
-  <si>
-    <t>▲ 137.67%</t>
-  </si>
-  <si>
-    <t>23-32</t>
-  </si>
-  <si>
-    <t>█████████  23</t>
-  </si>
-  <si>
-    <t>▼ -83.41%</t>
-  </si>
-  <si>
-    <t>Makeup</t>
-  </si>
-  <si>
-    <t>Blush</t>
-  </si>
-  <si>
-    <t>13-22</t>
-  </si>
-  <si>
-    <t>██████████ 26</t>
-  </si>
-  <si>
-    <t>➔ 0.45%</t>
-  </si>
-  <si>
-    <t>Lips</t>
-  </si>
-  <si>
-    <t>Liquid lipstick</t>
-  </si>
-  <si>
-    <t>43-52</t>
-  </si>
-  <si>
-    <t>▼ -66.43%</t>
-  </si>
-  <si>
-    <t>Nails</t>
-  </si>
-  <si>
-    <t>Top coat</t>
-  </si>
-  <si>
-    <t>█████      12</t>
-  </si>
-  <si>
-    <t>▼ -38.39%</t>
-  </si>
-  <si>
-    <t>Moisturizing treatment</t>
-  </si>
-  <si>
-    <t>Adults</t>
-  </si>
-  <si>
-    <t>33-42</t>
-  </si>
-  <si>
-    <t>████████   22</t>
-  </si>
-  <si>
-    <t>▼ -52.90%</t>
-  </si>
-  <si>
-    <t>Brow gel</t>
-  </si>
-  <si>
-    <t>████████   21</t>
-  </si>
-  <si>
-    <t>▼ -83.64%</t>
-  </si>
-  <si>
-    <t>Lip scrub</t>
-  </si>
-  <si>
-    <t>▲ 83.27%</t>
-  </si>
-  <si>
-    <t>Sun Protection</t>
-  </si>
-  <si>
-    <t>Sun protection gel</t>
-  </si>
-  <si>
-    <t>███████    17</t>
-  </si>
-  <si>
-    <t>▼ -79.53%</t>
-  </si>
-  <si>
-    <t>Matte lipstick</t>
-  </si>
-  <si>
-    <t>█████      13</t>
-  </si>
-  <si>
-    <t>▼ -45.19%</t>
-  </si>
-  <si>
-    <t>Body</t>
-  </si>
-  <si>
-    <t>Deodorant</t>
-  </si>
-  <si>
-    <t>▲ 22.00%</t>
-  </si>
-  <si>
-    <t>██████     16</t>
-  </si>
-  <si>
-    <t>▼ -60.41%</t>
+    <t>▲ 201.58%</t>
+  </si>
+  <si>
+    <t>▲ 20.48%</t>
+  </si>
+  <si>
+    <t>Nail treatment</t>
+  </si>
+  <si>
+    <t>██████████ 31</t>
+  </si>
+  <si>
+    <t>▲ 251.62%</t>
   </si>
   <si>
     <t>Total</t>
@@ -258,12 +240,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="9C0006"/>
+        <fgColor rgb="006100"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="006100"/>
+        <fgColor rgb="9C0006"/>
       </patternFill>
     </fill>
     <fill>
@@ -314,7 +296,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,7 +636,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="13" width="20" customWidth="1"/>
@@ -727,16 +709,16 @@
         <v>20</v>
       </c>
       <c r="I2">
-        <v>113.76</v>
+        <v>128.96</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="K2">
-        <v>150.57</v>
+        <v>120.99</v>
       </c>
       <c r="L2">
-        <v>2221.7400000000002</v>
+        <v>2790.74</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>22</v>
@@ -768,18 +750,18 @@
         <v>20</v>
       </c>
       <c r="I3">
-        <v>103.34</v>
+        <v>101.57</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K3">
-        <v>120.99</v>
+        <v>199.99</v>
       </c>
       <c r="L3">
-        <v>2281.16</v>
-      </c>
-      <c r="M3" s="4" t="s">
+        <v>3701.3900000000003</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -788,19 +770,19 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
@@ -809,19 +791,19 @@
         <v>20</v>
       </c>
       <c r="I4">
-        <v>103.19</v>
+        <v>104.96</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K4">
-        <v>23.99</v>
+        <v>100</v>
       </c>
       <c r="L4">
-        <v>654.96</v>
+        <v>1204.96</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -829,19 +811,19 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
         <v>19</v>
@@ -850,19 +832,19 @@
         <v>20</v>
       </c>
       <c r="I5">
-        <v>126.21</v>
+        <v>113.04</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K5">
-        <v>40.49</v>
+        <v>120.99</v>
       </c>
       <c r="L5">
-        <v>1178.95</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>36</v>
+        <v>2048.88</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -870,19 +852,19 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
@@ -891,19 +873,19 @@
         <v>20</v>
       </c>
       <c r="I6">
-        <v>60.96</v>
+        <v>107.09</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="K6">
-        <v>89.99</v>
+        <v>249.99</v>
       </c>
       <c r="L6">
-        <v>2130.73</v>
+        <v>4856.900000000001</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -911,19 +893,19 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
         <v>19</v>
@@ -932,19 +914,19 @@
         <v>20</v>
       </c>
       <c r="I7">
-        <v>138.79</v>
+        <v>97.8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="K7">
-        <v>149.99</v>
+        <v>103.99</v>
       </c>
       <c r="L7">
-        <v>1938.67</v>
+        <v>3113.51</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -952,19 +934,19 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -973,19 +955,19 @@
         <v>20</v>
       </c>
       <c r="I8">
-        <v>98.71</v>
+        <v>89.49</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K8">
-        <v>100</v>
+        <v>80.49</v>
       </c>
       <c r="L8">
-        <v>2298.71</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>49</v>
+        <v>1296.84</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -993,10 +975,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>25</v>
@@ -1005,7 +987,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>19</v>
@@ -1014,238 +996,115 @@
         <v>20</v>
       </c>
       <c r="I9" s="6">
-        <v>66.77</v>
+        <v>141.88</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="K9" s="6">
-        <v>20.99</v>
+        <v>47.99</v>
       </c>
       <c r="L9" s="6">
-        <v>507.55999999999995</v>
+        <v>1197.6599999999999</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="9" t="s">
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="9">
-        <v>68.78</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="9">
-        <v>103.99</v>
-      </c>
-      <c r="L10" s="9">
-        <v>2356.56</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>54</v>
+      <c r="I10" s="6">
+        <v>83.37</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10">
+        <v>150.57</v>
+      </c>
+      <c r="L10">
+        <v>3395.91</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="B11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="6">
-        <v>24.89</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11">
-        <v>59.99</v>
-      </c>
-      <c r="L11">
-        <v>1044.72</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>58</v>
+      <c r="I11" s="9">
+        <v>88.76</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="9">
+        <v>199.99</v>
+      </c>
+      <c r="L11" s="9">
+        <v>6288.450000000001</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12">
-        <v>46.23</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K12">
-        <v>40.49</v>
-      </c>
-      <c r="L12">
-        <v>572.6</v>
-      </c>
-      <c r="M12" s="3" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="9">
-        <v>166.76</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13">
-        <v>120.99</v>
-      </c>
-      <c r="L13">
-        <v>2344.58</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14">
-        <v>139.93</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K14">
-        <v>72.99</v>
-      </c>
-      <c r="L14">
-        <v>1307.77</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="1">
-        <f>SUM(I2:I14)</f>
-      </c>
-      <c r="J15" s="1">
-        <f>SUM(J2:J14)</f>
-      </c>
-      <c r="L15" s="1">
-        <f>SUM(L2:L14)</f>
+      <c r="I12" s="1">
+        <f>SUM(I2:I11)</f>
+      </c>
+      <c r="J12" s="1">
+        <f>SUM(J2:J11)</f>
+      </c>
+      <c r="L12" s="1">
+        <f>SUM(L2:L11)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>